<commit_message>
Nýjar skrár: doc/excel-skabalon.xlsx og measure_groups.py
</commit_message>
<xml_diff>
--- a/doc/excel-skabalon.xlsx
+++ b/doc/excel-skabalon.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonasson/voting/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04439718-2196-7F4B-A97E-A0B9B02ACE34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{01CCF48C-F532-CB49-81DB-632F0BC461D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4300" yWindow="-21100" windowWidth="37900" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4960" yWindow="-20940" windowWidth="38420" windowHeight="20900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Common settings" sheetId="2" r:id="rId1"/>
-    <sheet name="Quality measures" sheetId="3" r:id="rId2"/>
-    <sheet name="1-System-1" sheetId="1" r:id="rId3"/>
+    <sheet name="Quality measures" sheetId="4" r:id="rId2"/>
+    <sheet name="Votes shares" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="78">
   <si>
     <t>My reference votes</t>
   </si>
@@ -104,9 +104,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Votes and seats</t>
-  </si>
-  <si>
     <t>Number of simulations run</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>Avg. simulated values</t>
   </si>
   <si>
-    <t>Expected values</t>
-  </si>
-  <si>
     <t>Maximum values</t>
   </si>
   <si>
@@ -170,57 +164,15 @@
     <t>Standard deviations</t>
   </si>
   <si>
-    <t>Const</t>
-  </si>
-  <si>
-    <t>VoteShares</t>
-  </si>
-  <si>
     <t>Switching</t>
   </si>
   <si>
-    <t>Allocation with actual system for the reference votes</t>
-  </si>
-  <si>
-    <t>Electoral systems</t>
-  </si>
-  <si>
     <t>Individual lists</t>
   </si>
   <si>
     <t>Entropy (logarithmic)</t>
   </si>
   <si>
-    <t>Mininum allocation seat share</t>
-  </si>
-  <si>
-    <t>0.332</t>
-  </si>
-  <si>
-    <t>Pétur</t>
-  </si>
-  <si>
-    <t>Sum of differences of seats minus shares</t>
-  </si>
-  <si>
-    <t>Absolute values</t>
-  </si>
-  <si>
-    <t>Only positive values</t>
-  </si>
-  <si>
-    <t>Squared values</t>
-  </si>
-  <si>
-    <t>Sum absolute differences w.r.t. other seat specifications</t>
-  </si>
-  <si>
-    <t>Kristján</t>
-  </si>
-  <si>
-    <t>Sum absolute differences w.r.t. other electoral systems</t>
-  </si>
-  <si>
     <t>Only adjustment seats</t>
   </si>
   <si>
@@ -230,7 +182,91 @@
     <t>Party totals</t>
   </si>
   <si>
-    <t>Other quality indices</t>
+    <t>Values based on source votes</t>
+  </si>
+  <si>
+    <t>Optimal</t>
+  </si>
+  <si>
+    <t>Vote-shares</t>
+  </si>
+  <si>
+    <t>Icelandic-law</t>
+  </si>
+  <si>
+    <t>...</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>x,xxx</t>
+  </si>
+  <si>
+    <t>– compared with following electoral systems</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>xx</t>
+  </si>
+  <si>
+    <t>All constituencies combined</t>
+  </si>
+  <si>
+    <t>– compared with other seat specifications</t>
+  </si>
+  <si>
+    <t>Sum of absolute seat allocation differences:</t>
+  </si>
+  <si>
+    <t>Specific quality indices for seat allocations</t>
+  </si>
+  <si>
+    <t>Sum of squared values</t>
+  </si>
+  <si>
+    <t>Sum of positive values</t>
+  </si>
+  <si>
+    <t>Sum of absolute values</t>
+  </si>
+  <si>
+    <t>Allocated seats minus reference seat shares</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tested systems: </t>
+  </si>
+  <si>
+    <t>Kurtosis  for all simulations</t>
+  </si>
+  <si>
+    <t>Skewness  for all simulations</t>
+  </si>
+  <si>
+    <t>Standard deviations  for all simulations</t>
+  </si>
+  <si>
+    <t>Maxima for all simulations</t>
+  </si>
+  <si>
+    <t>Minima for all simulations</t>
+  </si>
+  <si>
+    <t>Average of indicated measures for all simulations</t>
+  </si>
+  <si>
+    <t>QUALITY MEASURES</t>
+  </si>
+  <si>
+    <t>– compared w. tested systems and source votes</t>
+  </si>
+  <si>
+    <t>Source votes and seats</t>
+  </si>
+  <si>
+    <t>Minimum reference seat share per seat</t>
   </si>
 </sst>
 </file>
@@ -242,7 +278,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,6 +342,55 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -327,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -379,9 +464,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -411,10 +493,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,10 +558,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -757,16 +881,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52CF09F3-0BAC-DA4E-845A-CDF8156E8D4F}">
-  <dimension ref="A1:W70"/>
+  <dimension ref="A1:W71"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView zoomScale="132" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.83203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="32.1640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="27.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="35.83203125" style="4" customWidth="1"/>
     <col min="3" max="3" width="9.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="2" customWidth="1"/>
     <col min="5" max="5" width="9.1640625" style="4" bestFit="1" customWidth="1"/>
@@ -790,129 +914,118 @@
       <c r="A1" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="29">
+      <c r="B1" s="28">
         <v>44452.446527777778</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="22"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A5" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="3">
-        <v>100</v>
-      </c>
+      <c r="B5" s="2"/>
       <c r="C5" s="4"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
+      </c>
+      <c r="B6" s="3">
+        <v>100</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
-    </row>
-    <row r="11" spans="1:23" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
-      <c r="B11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="T11" s="4"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
-      <c r="C12" s="13"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-      <c r="U12" s="9"/>
-      <c r="V12" s="9"/>
-      <c r="W12" s="9"/>
+    <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="6"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+    </row>
+    <row r="12" spans="1:23" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="38"/>
+      <c r="B12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="T12" s="4"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
@@ -946,50 +1059,50 @@
       <c r="V14" s="9"/>
       <c r="W14" s="9"/>
     </row>
-    <row r="16" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
-      <c r="V16" s="1"/>
-      <c r="W16" s="1"/>
-    </row>
-    <row r="17" spans="1:23" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="25"/>
-      <c r="B17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="T17" s="4"/>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
-      <c r="C18" s="13"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
-      <c r="U18" s="9"/>
-      <c r="V18" s="9"/>
-      <c r="W18" s="9"/>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15" s="7"/>
+      <c r="C15" s="13"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="9"/>
+      <c r="W15" s="9"/>
+    </row>
+    <row r="17" spans="1:23" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="6"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+    </row>
+    <row r="18" spans="1:23" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="24"/>
+      <c r="B18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="T18" s="4"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
@@ -1023,50 +1136,50 @@
       <c r="V20" s="9"/>
       <c r="W20" s="9"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A22" s="6"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
-      <c r="T22" s="1"/>
-      <c r="U22" s="1"/>
-      <c r="V22" s="1"/>
-      <c r="W22" s="1"/>
-    </row>
-    <row r="23" spans="1:23" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="25"/>
-      <c r="B23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="O23" s="4"/>
-      <c r="T23" s="4"/>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A24" s="6"/>
-      <c r="C24" s="13"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-      <c r="P24" s="10"/>
-      <c r="Q24" s="10"/>
-      <c r="R24" s="10"/>
-      <c r="U24" s="9"/>
-      <c r="V24" s="9"/>
-      <c r="W24" s="9"/>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A21" s="6"/>
+      <c r="C21" s="13"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="9"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A23" s="6"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+    </row>
+    <row r="24" spans="1:23" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="24"/>
+      <c r="B24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="T24" s="4"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
@@ -1100,50 +1213,50 @@
       <c r="V26" s="9"/>
       <c r="W26" s="9"/>
     </row>
-    <row r="28" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="6"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
-      <c r="Q28" s="1"/>
-      <c r="R28" s="1"/>
-      <c r="T28" s="1"/>
-      <c r="U28" s="1"/>
-      <c r="V28" s="1"/>
-      <c r="W28" s="1"/>
-    </row>
-    <row r="29" spans="1:23" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="25"/>
-      <c r="B29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="T29" s="4"/>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A30" s="6"/>
-      <c r="C30" s="13"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="K30" s="21"/>
-      <c r="L30" s="21"/>
-      <c r="M30" s="10"/>
-      <c r="P30" s="10"/>
-      <c r="Q30" s="10"/>
-      <c r="R30" s="10"/>
-      <c r="U30" s="9"/>
-      <c r="V30" s="9"/>
-      <c r="W30" s="9"/>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A27" s="6"/>
+      <c r="C27" s="13"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+      <c r="U27" s="9"/>
+      <c r="V27" s="9"/>
+      <c r="W27" s="9"/>
+    </row>
+    <row r="29" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="6"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+    </row>
+    <row r="30" spans="1:23" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="24"/>
+      <c r="B30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="T30" s="4"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
@@ -1151,7 +1264,7 @@
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
-      <c r="K31" s="10"/>
+      <c r="K31" s="21"/>
       <c r="L31" s="21"/>
       <c r="M31" s="10"/>
       <c r="P31" s="10"/>
@@ -1177,49 +1290,50 @@
       <c r="V32" s="9"/>
       <c r="W32" s="9"/>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A34" s="6"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="1"/>
-      <c r="R34" s="1"/>
-      <c r="T34" s="1"/>
-      <c r="U34" s="1"/>
-      <c r="V34" s="1"/>
-      <c r="W34" s="1"/>
-    </row>
-    <row r="35" spans="1:23" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="25"/>
-      <c r="B35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="O35" s="4"/>
-      <c r="T35" s="4"/>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A36" s="6"/>
-      <c r="C36" s="13"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="22"/>
-      <c r="K36" s="10"/>
-      <c r="L36" s="10"/>
-      <c r="M36" s="22"/>
-      <c r="P36" s="10"/>
-      <c r="Q36" s="10"/>
-      <c r="R36" s="22"/>
-      <c r="U36" s="9"/>
-      <c r="V36" s="9"/>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A33" s="6"/>
+      <c r="C33" s="13"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="21"/>
+      <c r="M33" s="10"/>
+      <c r="P33" s="10"/>
+      <c r="Q33" s="10"/>
+      <c r="R33" s="10"/>
+      <c r="U33" s="9"/>
+      <c r="V33" s="9"/>
+      <c r="W33" s="9"/>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A35" s="6"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+      <c r="T35" s="1"/>
+      <c r="U35" s="1"/>
+      <c r="V35" s="1"/>
+      <c r="W35" s="1"/>
+    </row>
+    <row r="36" spans="1:23" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="24"/>
+      <c r="B36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="T36" s="4"/>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A37" s="6"/>
@@ -1251,54 +1365,57 @@
       <c r="U38" s="9"/>
       <c r="V38" s="9"/>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A40" s="6"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
-      <c r="O40" s="1"/>
-      <c r="P40" s="1"/>
-      <c r="Q40" s="1"/>
-      <c r="R40" s="1"/>
-      <c r="T40" s="1"/>
-      <c r="U40" s="1"/>
-      <c r="V40" s="1"/>
-      <c r="W40" s="1"/>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A39" s="6"/>
+      <c r="C39" s="13"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="22"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="10"/>
+      <c r="M39" s="22"/>
+      <c r="P39" s="10"/>
+      <c r="Q39" s="10"/>
+      <c r="R39" s="22"/>
+      <c r="U39" s="9"/>
+      <c r="V39" s="9"/>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41" s="6"/>
-      <c r="C41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
-      <c r="K41" s="5"/>
-      <c r="L41" s="5"/>
-      <c r="M41" s="5"/>
-      <c r="P41" s="5"/>
-      <c r="Q41" s="5"/>
-      <c r="R41" s="5"/>
-      <c r="U41" s="5"/>
-      <c r="V41" s="5"/>
-      <c r="W41" s="5"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="1"/>
+      <c r="T41" s="1"/>
+      <c r="U41" s="1"/>
+      <c r="V41" s="1"/>
+      <c r="W41" s="1"/>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A42" s="6"/>
-      <c r="C42" s="13"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="K42" s="10"/>
-      <c r="L42" s="10"/>
-      <c r="P42" s="10"/>
-      <c r="Q42" s="10"/>
-      <c r="U42" s="9"/>
-      <c r="V42" s="9"/>
+      <c r="C42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5"/>
+      <c r="P42" s="5"/>
+      <c r="Q42" s="5"/>
+      <c r="R42" s="5"/>
+      <c r="U42" s="5"/>
+      <c r="V42" s="5"/>
+      <c r="W42" s="5"/>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A43" s="6"/>
@@ -1324,54 +1441,54 @@
       <c r="U44" s="9"/>
       <c r="V44" s="9"/>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A46" s="6"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
-      <c r="L46" s="1"/>
-      <c r="M46" s="1"/>
-      <c r="O46" s="1"/>
-      <c r="P46" s="1"/>
-      <c r="Q46" s="1"/>
-      <c r="R46" s="1"/>
-      <c r="T46" s="1"/>
-      <c r="U46" s="1"/>
-      <c r="V46" s="1"/>
-      <c r="W46" s="1"/>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A45" s="6"/>
+      <c r="C45" s="13"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="K45" s="10"/>
+      <c r="L45" s="10"/>
+      <c r="P45" s="10"/>
+      <c r="Q45" s="10"/>
+      <c r="U45" s="9"/>
+      <c r="V45" s="9"/>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>
-      <c r="C47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
-      <c r="K47" s="5"/>
-      <c r="L47" s="5"/>
-      <c r="M47" s="5"/>
-      <c r="P47" s="5"/>
-      <c r="Q47" s="5"/>
-      <c r="R47" s="5"/>
-      <c r="U47" s="5"/>
-      <c r="V47" s="5"/>
-      <c r="W47" s="5"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="1"/>
+      <c r="R47" s="1"/>
+      <c r="T47" s="1"/>
+      <c r="U47" s="1"/>
+      <c r="V47" s="1"/>
+      <c r="W47" s="1"/>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A48" s="6"/>
-      <c r="C48" s="13"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="10"/>
-      <c r="K48" s="10"/>
-      <c r="L48" s="10"/>
-      <c r="P48" s="10"/>
-      <c r="Q48" s="10"/>
-      <c r="U48" s="9"/>
-      <c r="V48" s="9"/>
+      <c r="C48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
+      <c r="P48" s="5"/>
+      <c r="Q48" s="5"/>
+      <c r="R48" s="5"/>
+      <c r="U48" s="5"/>
+      <c r="V48" s="5"/>
+      <c r="W48" s="5"/>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A49" s="6"/>
@@ -1397,17 +1514,26 @@
       <c r="U50" s="9"/>
       <c r="V50" s="9"/>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A52" s="14"/>
-    </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A54" s="15"/>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A51" s="6"/>
+      <c r="C51" s="13"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="K51" s="10"/>
+      <c r="L51" s="10"/>
+      <c r="P51" s="10"/>
+      <c r="Q51" s="10"/>
+      <c r="U51" s="9"/>
+      <c r="V51" s="9"/>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A53" s="14"/>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A55" s="17"/>
+      <c r="A55" s="15"/>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A56" s="16"/>
+      <c r="A56" s="17"/>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A57" s="16"/>
@@ -1419,10 +1545,10 @@
       <c r="A59" s="16"/>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A60" s="17"/>
+      <c r="A60" s="16"/>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A61" s="16"/>
+      <c r="A61" s="17"/>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A62" s="16"/>
@@ -1431,25 +1557,28 @@
       <c r="A63" s="16"/>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A64" s="15"/>
+      <c r="A64" s="16"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" s="16"/>
+      <c r="A65" s="15"/>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" s="16"/>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" s="15"/>
+      <c r="A67" s="16"/>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" s="16"/>
+      <c r="A68" s="15"/>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" s="16"/>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" s="16"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1457,395 +1586,1071 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16C1E315-7991-8245-BCCD-6560DB3C071A}">
-  <dimension ref="A1:F34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748E841B-6C29-834D-9376-1530C4084D09}">
+  <dimension ref="A1:AB38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="174" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="172" zoomScaleNormal="142" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="57.5" customWidth="1"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.83203125" customWidth="1"/>
+    <col min="7" max="7" width="3.6640625" customWidth="1"/>
+    <col min="12" max="12" width="4" customWidth="1"/>
+    <col min="17" max="17" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="14"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="14"/>
-      <c r="B2" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="14" t="s">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A1" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="R1" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="W1" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB1" s="27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B2" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="N2" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="O2" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="P2" s="55" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A3" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="56"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A4" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="40"/>
+      <c r="C4" s="48">
+        <v>11.57374961438035</v>
+      </c>
+      <c r="D4" s="48">
+        <v>11.320168549521201</v>
+      </c>
+      <c r="E4" s="48">
+        <v>11.320168549521201</v>
+      </c>
+      <c r="F4" s="48">
+        <v>11.320168549521201</v>
+      </c>
+      <c r="H4" s="48">
+        <v>11.320168549521201</v>
+      </c>
+      <c r="I4" s="48">
+        <v>11.57374961438035</v>
+      </c>
+      <c r="J4" s="48">
+        <v>11.320168549521201</v>
+      </c>
+      <c r="K4" s="48">
+        <v>11.320168549521201</v>
+      </c>
+      <c r="M4" s="48">
+        <v>12.321</v>
+      </c>
+      <c r="N4" s="48">
+        <v>11.57374961438035</v>
+      </c>
+      <c r="O4" s="48">
+        <v>11.320168549521201</v>
+      </c>
+      <c r="P4" s="48">
+        <v>11.320168549521201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A5" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="40"/>
+      <c r="C5" s="48">
+        <v>8.7096683505766102</v>
+      </c>
+      <c r="D5" s="48">
+        <v>7.5220884798964747</v>
+      </c>
+      <c r="E5" s="48">
+        <v>7.5220884798964747</v>
+      </c>
+      <c r="F5" s="48">
+        <v>8.4491938244714255</v>
+      </c>
+      <c r="H5" s="48">
+        <v>8.4491938244714255</v>
+      </c>
+      <c r="I5" s="48">
+        <v>8.7096683505766102</v>
+      </c>
+      <c r="J5" s="48">
+        <v>7.5220884798964747</v>
+      </c>
+      <c r="K5" s="48">
+        <v>7.5220884798964747</v>
+      </c>
+      <c r="M5" s="48">
+        <v>8.4491938244714255</v>
+      </c>
+      <c r="N5" s="48">
+        <v>8.7096683505766102</v>
+      </c>
+      <c r="O5" s="48">
+        <v>7.5220884798964747</v>
+      </c>
+      <c r="P5" s="48">
+        <v>7.5220884798964747</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A6" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="40"/>
+      <c r="C6" s="48">
+        <v>5.3656269308088378</v>
+      </c>
+      <c r="D6" s="48">
+        <v>5.1574152328218332</v>
+      </c>
+      <c r="E6" s="48">
+        <v>5.1574152328218332</v>
+      </c>
+      <c r="F6" s="48">
+        <v>5.4636800423991536</v>
+      </c>
+      <c r="H6" s="48">
+        <v>5.4636800423991536</v>
+      </c>
+      <c r="I6" s="48">
+        <v>5.3656269308088378</v>
+      </c>
+      <c r="J6" s="48">
+        <v>5.1574152328218332</v>
+      </c>
+      <c r="K6" s="48">
+        <v>5.1574152328218332</v>
+      </c>
+      <c r="M6" s="48">
+        <v>5.4636800423991536</v>
+      </c>
+      <c r="N6" s="48">
+        <v>5.3656269308088378</v>
+      </c>
+      <c r="O6" s="48">
+        <v>5.1574152328218332</v>
+      </c>
+      <c r="P6" s="48">
+        <v>5.1574152328218332</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B7" s="40"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="39"/>
+      <c r="O7" s="39"/>
+      <c r="P7" s="39"/>
+    </row>
+    <row r="8" spans="1:28" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="14"/>
+    </row>
+    <row r="9" spans="1:28" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C9" s="48">
+        <v>502.48786328356698</v>
+      </c>
+      <c r="D9" s="48">
+        <v>500.51864530656098</v>
+      </c>
+      <c r="E9" s="48">
+        <v>500.51864530656098</v>
+      </c>
+      <c r="F9" s="48">
+        <v>500.27496646630999</v>
+      </c>
+      <c r="H9" s="48">
+        <v>500.27496646630999</v>
+      </c>
+      <c r="I9" s="48">
+        <v>502.48786328356698</v>
+      </c>
+      <c r="J9" s="48">
+        <v>500.51864530656098</v>
+      </c>
+      <c r="K9" s="48">
+        <v>500.51864530656098</v>
+      </c>
+      <c r="M9" s="48">
+        <v>500.27496646630999</v>
+      </c>
+      <c r="N9" s="48">
+        <v>502.48786328356698</v>
+      </c>
+      <c r="O9" s="48">
+        <v>500.51864530656098</v>
+      </c>
+      <c r="P9" s="48">
+        <v>500.51864530656098</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="48">
+        <v>0.2906195571037572</v>
+      </c>
+      <c r="D10" s="48">
+        <v>0.30533393774554252</v>
+      </c>
+      <c r="E10" s="48">
+        <v>0.30533393774554252</v>
+      </c>
+      <c r="F10" s="48">
+        <v>0.33200000000000002</v>
+      </c>
+      <c r="H10" s="48">
+        <v>0.33200000000000002</v>
+      </c>
+      <c r="I10" s="48">
+        <v>0.2906195571037572</v>
+      </c>
+      <c r="J10" s="48">
+        <v>0.30533393774554252</v>
+      </c>
+      <c r="K10" s="48">
+        <v>0.30533393774554252</v>
+      </c>
+      <c r="M10" s="48">
+        <v>0.33200000000000002</v>
+      </c>
+      <c r="N10" s="48">
+        <v>0.2906195571037572</v>
+      </c>
+      <c r="O10" s="48">
+        <v>0.30533393774554252</v>
+      </c>
+      <c r="P10" s="48">
+        <v>0.30533393774554252</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A12" s="54" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A13" s="27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A14" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="C14" s="48">
+        <v>0.16969778979579775</v>
+      </c>
+      <c r="D14" s="48">
+        <v>0.58796874354890705</v>
+      </c>
+      <c r="E14" s="48">
+        <v>0.58796874354890705</v>
+      </c>
+      <c r="F14" s="48">
+        <v>1.9013408502497553E-2</v>
+      </c>
+      <c r="H14" s="39">
+        <v>1</v>
+      </c>
+      <c r="I14" s="39">
+        <v>0</v>
+      </c>
+      <c r="J14" s="39">
+        <v>0</v>
+      </c>
+      <c r="K14" s="39">
+        <v>0</v>
+      </c>
+      <c r="M14" s="39">
+        <v>1</v>
+      </c>
+      <c r="N14" s="39">
+        <v>1</v>
+      </c>
+      <c r="O14" s="39">
+        <v>1</v>
+      </c>
+      <c r="P14" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A15" s="40"/>
+      <c r="B15" s="40" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
+      <c r="C15" s="48">
+        <v>2.5982710939639166</v>
+      </c>
+      <c r="D15" s="48">
+        <v>2.2242663752117666</v>
+      </c>
+      <c r="E15" s="48">
+        <v>2.2242663752117666</v>
+      </c>
+      <c r="F15" s="48">
+        <v>2.7946825911161115</v>
+      </c>
+      <c r="H15" s="39">
+        <v>2</v>
+      </c>
+      <c r="I15" s="39">
+        <v>2</v>
+      </c>
+      <c r="J15" s="39">
+        <v>2</v>
+      </c>
+      <c r="K15" s="39">
+        <v>2</v>
+      </c>
+      <c r="M15" s="39">
+        <v>2</v>
+      </c>
+      <c r="N15" s="39">
+        <v>2</v>
+      </c>
+      <c r="O15" s="39">
+        <v>2</v>
+      </c>
+      <c r="P15" s="39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A16" s="52" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="48">
+        <v>0.19814000668899046</v>
+      </c>
+      <c r="D16" s="48">
+        <v>0.18311117514784481</v>
+      </c>
+      <c r="E16" s="48">
+        <v>0.18311117514784481</v>
+      </c>
+      <c r="F16" s="48">
+        <v>0.78679779805232808</v>
+      </c>
+      <c r="H16" s="39">
+        <v>0</v>
+      </c>
+      <c r="I16" s="39">
+        <v>1</v>
+      </c>
+      <c r="J16" s="39">
+        <v>0</v>
+      </c>
+      <c r="K16" s="39">
+        <v>0</v>
+      </c>
+      <c r="M16" s="39">
+        <v>2</v>
+      </c>
+      <c r="N16" s="39">
+        <v>3</v>
+      </c>
+      <c r="O16" s="39">
+        <v>2</v>
+      </c>
+      <c r="P16" s="39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B17" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="48">
+        <v>2.7721850223762061</v>
+      </c>
+      <c r="D17" s="48">
+        <v>2.2357729203279417</v>
+      </c>
+      <c r="E17" s="48">
+        <v>2.2357729203279417</v>
+      </c>
+      <c r="F17" s="48">
+        <v>2.1930189033620926</v>
+      </c>
+      <c r="H17" s="39">
+        <v>2</v>
+      </c>
+      <c r="I17" s="39">
+        <v>2</v>
+      </c>
+      <c r="J17" s="39">
+        <v>2</v>
+      </c>
+      <c r="K17" s="39">
+        <v>2</v>
+      </c>
+      <c r="M17" s="39">
+        <v>2</v>
+      </c>
+      <c r="N17" s="39">
+        <v>2</v>
+      </c>
+      <c r="O17" s="39">
+        <v>2</v>
+      </c>
+      <c r="P17" s="39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B18" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="D18" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="I18" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="J18" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="K18" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="M18" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="N18" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="O18" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="P18" s="39" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B19" s="40"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="39"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="39"/>
+      <c r="O19" s="39"/>
+      <c r="P19" s="39"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A20" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="13">
-        <v>11.320168549521201</v>
-      </c>
-      <c r="C6" s="13">
-        <v>11.57374961438035</v>
-      </c>
-      <c r="D6" s="13">
-        <v>11.320168549521201</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" s="13">
-        <v>8.4491938244714255</v>
-      </c>
-      <c r="C7" s="13">
-        <v>8.7096683505766102</v>
-      </c>
-      <c r="D7" s="13">
-        <v>7.5220884798964747</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="39"/>
+      <c r="M20" s="39"/>
+      <c r="N20" s="39"/>
+      <c r="O20" s="39"/>
+      <c r="P20" s="39"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A21" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" s="51">
+        <v>0.121</v>
+      </c>
+      <c r="E21" s="51">
+        <v>0.44606235918925974</v>
+      </c>
+      <c r="F21" s="51">
+        <v>3.6810559144514143E-2</v>
+      </c>
+      <c r="H21" s="50">
+        <v>0</v>
+      </c>
+      <c r="I21" s="50">
+        <v>0</v>
+      </c>
+      <c r="J21" s="50">
+        <v>0</v>
+      </c>
+      <c r="K21" s="50">
+        <v>1</v>
+      </c>
+      <c r="L21" s="50"/>
+      <c r="M21" s="50">
+        <v>0</v>
+      </c>
+      <c r="N21" s="50">
+        <v>3</v>
+      </c>
+      <c r="O21" s="50">
+        <v>2</v>
+      </c>
+      <c r="P21" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B22" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="48">
+        <v>0.121</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="H22" s="39">
+        <v>0</v>
+      </c>
+      <c r="I22" s="39">
+        <v>0</v>
+      </c>
+      <c r="J22" s="39">
+        <v>0</v>
+      </c>
+      <c r="K22" s="39">
+        <v>1</v>
+      </c>
+      <c r="M22" s="39">
+        <v>3</v>
+      </c>
+      <c r="N22" s="39">
+        <v>0</v>
+      </c>
+      <c r="O22" s="39">
+        <v>3</v>
+      </c>
+      <c r="P22" s="39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B23" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="48">
+        <v>3.6810559144514143E-2</v>
+      </c>
+      <c r="D23" s="48">
+        <v>0.8932948068518588</v>
+      </c>
+      <c r="E23">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23" s="39">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <v>2</v>
+      </c>
+      <c r="O23">
+        <v>3</v>
+      </c>
+      <c r="P23" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B24" s="14" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B8" s="13">
-        <v>5.4636800423991536</v>
-      </c>
-      <c r="C8" s="13">
-        <v>5.3656269308088378</v>
-      </c>
-      <c r="D8" s="13">
-        <v>5.1574152328218332</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="28" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="C24" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="I24" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="J24" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="K24" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="L24" s="39"/>
+      <c r="M24" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="N24" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="O24" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="P24" s="39" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A25" s="52" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="49">
+        <v>0</v>
+      </c>
+      <c r="D25" s="51">
+        <v>0.34612668354933307</v>
+      </c>
+      <c r="E25" s="51">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="F25" s="51">
+        <v>0.49345681797586316</v>
+      </c>
+      <c r="H25" s="50">
+        <v>0</v>
+      </c>
+      <c r="I25" s="50">
+        <v>0</v>
+      </c>
+      <c r="J25" s="50">
+        <v>2</v>
+      </c>
+      <c r="K25" s="50">
+        <v>0</v>
+      </c>
+      <c r="L25" s="50"/>
+      <c r="M25" s="50">
+        <v>0</v>
+      </c>
+      <c r="N25" s="50">
+        <v>2</v>
+      </c>
+      <c r="O25" s="50">
+        <v>2</v>
+      </c>
+      <c r="P25" s="50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B26" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="13">
-        <v>500.27496646630999</v>
-      </c>
-      <c r="C11" s="13">
-        <v>502.48786328356698</v>
-      </c>
-      <c r="D11" s="13">
-        <v>500.51864530656098</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="13">
-        <v>0.2906195571037572</v>
-      </c>
-      <c r="D12" s="13">
-        <v>0.30533393774554252</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="F14" s="39"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="40" t="s">
+      <c r="C26" s="48">
+        <v>0.34612668354933307</v>
+      </c>
+      <c r="D26" s="49">
+        <v>0</v>
+      </c>
+      <c r="E26" s="48">
+        <v>2.4569999999999999</v>
+      </c>
+      <c r="F26" s="48">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="H26" s="49">
+        <v>0</v>
+      </c>
+      <c r="I26" s="49">
+        <v>0</v>
+      </c>
+      <c r="J26" s="49">
+        <v>2</v>
+      </c>
+      <c r="K26" s="49">
+        <v>1</v>
+      </c>
+      <c r="L26" s="50"/>
+      <c r="M26" s="49">
+        <v>2</v>
+      </c>
+      <c r="N26" s="49">
+        <v>0</v>
+      </c>
+      <c r="O26" s="49">
+        <v>2</v>
+      </c>
+      <c r="P26" s="49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B27" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="5">
-        <v>0</v>
-      </c>
-      <c r="C16" s="5">
-        <v>0</v>
-      </c>
-      <c r="D16" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" s="5">
-        <v>2</v>
-      </c>
-      <c r="C17" s="5">
-        <v>2</v>
-      </c>
-      <c r="D17" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="39" t="s">
-        <v>64</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B19" s="5">
-        <v>0</v>
-      </c>
-      <c r="C19" s="5">
-        <v>0</v>
-      </c>
-      <c r="D19" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" s="5">
-        <v>2</v>
-      </c>
-      <c r="C20" s="5">
-        <v>2</v>
-      </c>
-      <c r="D20" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="5">
-        <v>0</v>
-      </c>
-      <c r="C24" s="5">
-        <v>0</v>
-      </c>
-      <c r="D24" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="5">
-        <v>0</v>
-      </c>
-      <c r="C25" s="5">
-        <v>0</v>
-      </c>
-      <c r="D25" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="5">
-        <v>0</v>
-      </c>
-      <c r="C26" s="5">
-        <v>0</v>
-      </c>
-      <c r="D26" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="39" t="s">
-        <v>64</v>
-      </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B28" s="5">
-        <v>0</v>
-      </c>
-      <c r="C28" s="5">
-        <v>0</v>
-      </c>
-      <c r="D28" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B29" s="5">
-        <v>2</v>
-      </c>
-      <c r="C29" s="5">
-        <v>2</v>
-      </c>
-      <c r="D29" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B30" s="5">
-        <v>0</v>
-      </c>
-      <c r="C30" s="5">
-        <v>0</v>
-      </c>
-      <c r="D30" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
+      <c r="C27" s="48">
+        <v>0.49345681797586316</v>
+      </c>
+      <c r="D27" s="48">
+        <v>0.84746134572101128</v>
+      </c>
+      <c r="E27" s="48">
+        <v>2.4565424329266676</v>
+      </c>
+      <c r="F27" s="49">
+        <v>0</v>
+      </c>
+      <c r="H27" s="49">
+        <v>0</v>
+      </c>
+      <c r="I27" s="49">
+        <v>1</v>
+      </c>
+      <c r="J27" s="49">
+        <v>0</v>
+      </c>
+      <c r="K27" s="49">
+        <v>0</v>
+      </c>
+      <c r="L27" s="50"/>
+      <c r="M27" s="49">
+        <v>3</v>
+      </c>
+      <c r="N27" s="49">
+        <v>3</v>
+      </c>
+      <c r="O27" s="49">
+        <v>4</v>
+      </c>
+      <c r="P27" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B28" s="14"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="39"/>
+      <c r="M28" s="39"/>
+      <c r="N28" s="39"/>
+      <c r="O28" s="39"/>
+      <c r="P28" s="39"/>
+      <c r="R28" s="39"/>
+      <c r="S28" s="39"/>
+      <c r="T28" s="39"/>
+      <c r="U28" s="39"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A29" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="40"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="48"/>
+      <c r="F29" s="48"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="39"/>
+      <c r="M29" s="39"/>
+      <c r="N29" s="39"/>
+      <c r="O29" s="39"/>
+      <c r="P29" s="39"/>
+    </row>
+    <row r="30" spans="1:21" s="22" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="45"/>
+      <c r="C30" s="44">
+        <v>7.3345721486019477E-2</v>
+      </c>
+      <c r="D30" s="44">
+        <v>0.37588227455947576</v>
+      </c>
+      <c r="E30" s="44">
+        <v>0.37588227455947576</v>
+      </c>
+      <c r="F30" s="44">
+        <v>5.0892136616471073E-2</v>
+      </c>
+      <c r="G30" s="43"/>
+      <c r="H30" s="43">
+        <v>0</v>
+      </c>
+      <c r="I30" s="43">
+        <v>1</v>
+      </c>
+      <c r="J30" s="43">
+        <v>0</v>
+      </c>
+      <c r="K30" s="43">
+        <v>0</v>
+      </c>
+      <c r="L30" s="42"/>
+      <c r="M30" s="43">
+        <v>2</v>
+      </c>
+      <c r="N30" s="43">
+        <v>1</v>
+      </c>
+      <c r="O30" s="43">
+        <v>3</v>
+      </c>
+      <c r="P30" s="43">
+        <v>3</v>
+      </c>
+      <c r="Q30" s="42"/>
+    </row>
+    <row r="31" spans="1:21" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="B32" s="5">
-        <v>6</v>
-      </c>
-      <c r="C32" s="5">
-        <v>8</v>
-      </c>
-      <c r="D32" s="5">
-        <v>8</v>
-      </c>
-      <c r="F32" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33" s="5">
-        <v>0</v>
-      </c>
-      <c r="C33" s="5">
-        <v>0</v>
-      </c>
-      <c r="D33" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
+      <c r="B31" s="45"/>
+      <c r="C31" s="44">
+        <v>0.83021769396323619</v>
+      </c>
+      <c r="D31" s="44">
+        <v>0.90006631200155518</v>
+      </c>
+      <c r="E31" s="44">
+        <v>0.90006631200155518</v>
+      </c>
+      <c r="F31" s="44">
+        <v>0.5962960523233668</v>
+      </c>
+      <c r="G31" s="42"/>
+      <c r="H31" s="43">
+        <v>1</v>
+      </c>
+      <c r="I31" s="43">
+        <v>0</v>
+      </c>
+      <c r="J31" s="43">
+        <v>1</v>
+      </c>
+      <c r="K31" s="43">
+        <v>1</v>
+      </c>
+      <c r="L31" s="42"/>
+      <c r="M31" s="43">
+        <v>1</v>
+      </c>
+      <c r="N31" s="43">
+        <v>2</v>
+      </c>
+      <c r="O31" s="43">
+        <v>3</v>
+      </c>
+      <c r="P31" s="43">
+        <v>3</v>
+      </c>
+      <c r="Q31" s="42"/>
+      <c r="R31" s="41"/>
+      <c r="S31" s="41"/>
+      <c r="T31" s="41"/>
+      <c r="U31" s="41"/>
+    </row>
+    <row r="32" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R32" s="39"/>
+      <c r="S32" s="39"/>
+      <c r="T32" s="39"/>
+      <c r="U32" s="39"/>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="R33" s="39"/>
+      <c r="S33" s="39"/>
+      <c r="T33" s="39"/>
+      <c r="U33" s="39"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A35" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="5">
-        <v>0</v>
-      </c>
-      <c r="C34" s="5">
-        <v>0</v>
-      </c>
-      <c r="D34" s="5">
-        <v>0</v>
-      </c>
-      <c r="F34" t="s">
-        <v>54</v>
-      </c>
+      <c r="C35" s="39">
+        <v>0</v>
+      </c>
+      <c r="D35" s="39">
+        <v>0</v>
+      </c>
+      <c r="E35" s="39">
+        <v>0</v>
+      </c>
+      <c r="F35" s="39">
+        <v>0</v>
+      </c>
+      <c r="R35" s="39"/>
+      <c r="S35" s="39"/>
+      <c r="T35" s="39"/>
+      <c r="U35" s="39"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A38" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1853,17 +2658,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB50"/>
   <sheetViews>
-    <sheetView zoomScale="138" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="10" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19" style="4" customWidth="1"/>
     <col min="3" max="4" width="10" style="2" customWidth="1"/>
     <col min="5" max="5" width="10.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.6640625" style="2" customWidth="1"/>
@@ -1894,21 +2699,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="32" t="s">
+      <c r="A1" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="28"/>
+      <c r="D1" s="27"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="C2" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="28"/>
-      <c r="G2" s="31" t="s">
-        <v>34</v>
+      <c r="C2" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="27"/>
+      <c r="G2" s="30" t="s">
+        <v>33</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -1916,13 +2721,13 @@
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="30">
+        <v>32</v>
+      </c>
+      <c r="G3" s="29">
         <v>0</v>
       </c>
       <c r="H3" s="1"/>
@@ -1934,13 +2739,13 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="30">
+      <c r="G4" s="29">
         <v>0.05</v>
       </c>
       <c r="H4" s="1"/>
@@ -1952,13 +2757,15 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="23"/>
+      <c r="G5" s="29">
+        <v>0</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -1978,13 +2785,13 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="31"/>
+        <v>35</v>
+      </c>
+      <c r="G7" s="30"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -2004,8 +2811,8 @@
       <c r="Q8" s="3"/>
     </row>
     <row r="9" spans="1:28" ht="17" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
-        <v>39</v>
+      <c r="A9" s="32" t="s">
+        <v>38</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="1" t="s">
@@ -2024,23 +2831,23 @@
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
-      <c r="M9" s="34"/>
+      <c r="M9" s="33"/>
       <c r="N9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
-      <c r="Q9" s="34"/>
+      <c r="Q9" s="33"/>
       <c r="R9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="S9" s="1"/>
-      <c r="T9" s="34"/>
+      <c r="T9" s="33"/>
       <c r="V9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W9" s="1"/>
-      <c r="X9" s="34"/>
+      <c r="X9" s="33"/>
       <c r="Z9" s="1" t="s">
         <v>15</v>
       </c>
@@ -2070,7 +2877,7 @@
       <c r="K10" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="L10" s="35" t="s">
+      <c r="L10" s="34" t="s">
         <v>4</v>
       </c>
       <c r="N10" s="23" t="s">
@@ -2079,7 +2886,7 @@
       <c r="O10" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="P10" s="35" t="s">
+      <c r="P10" s="34" t="s">
         <v>4</v>
       </c>
       <c r="R10" s="23" t="s">
@@ -2088,7 +2895,7 @@
       <c r="S10" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="T10" s="35" t="s">
+      <c r="T10" s="34" t="s">
         <v>4</v>
       </c>
       <c r="V10" s="23" t="s">
@@ -2097,7 +2904,7 @@
       <c r="W10" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="X10" s="35" t="s">
+      <c r="X10" s="34" t="s">
         <v>4</v>
       </c>
       <c r="Z10" s="23" t="s">
@@ -2109,10 +2916,10 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="8">
         <v>1500</v>
@@ -2316,10 +3123,10 @@
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="8">
         <v>1526.22</v>
@@ -2381,7 +3188,7 @@
       <c r="AB15" s="9"/>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A16" s="25"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="4" t="s">
         <v>6</v>
       </c>
@@ -2523,7 +3330,7 @@
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>5</v>
@@ -2558,7 +3365,7 @@
       <c r="O19" s="8">
         <v>8</v>
       </c>
-      <c r="P19" s="36">
+      <c r="P19" s="35">
         <v>10</v>
       </c>
       <c r="Q19" s="8"/>
@@ -2568,7 +3375,7 @@
       <c r="S19" s="8">
         <v>2</v>
       </c>
-      <c r="T19" s="36">
+      <c r="T19" s="35">
         <v>2</v>
       </c>
       <c r="U19" s="8"/>
@@ -2590,7 +3397,7 @@
       <c r="AB19" s="9"/>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A20" s="25"/>
+      <c r="A20" s="24"/>
       <c r="B20" s="4" t="s">
         <v>6</v>
       </c>
@@ -2624,7 +3431,7 @@
       <c r="O20" s="8">
         <v>7</v>
       </c>
-      <c r="P20" s="36">
+      <c r="P20" s="35">
         <v>10</v>
       </c>
       <c r="Q20" s="8"/>
@@ -2634,7 +3441,7 @@
       <c r="S20" s="8">
         <v>2</v>
       </c>
-      <c r="T20" s="36">
+      <c r="T20" s="35">
         <v>3</v>
       </c>
       <c r="U20" s="8"/>
@@ -2690,7 +3497,7 @@
       <c r="O21" s="8">
         <v>14</v>
       </c>
-      <c r="P21" s="36">
+      <c r="P21" s="35">
         <v>20</v>
       </c>
       <c r="Q21" s="8"/>
@@ -2700,7 +3507,7 @@
       <c r="S21" s="8">
         <v>3</v>
       </c>
-      <c r="T21" s="36">
+      <c r="T21" s="35">
         <v>5</v>
       </c>
       <c r="U21" s="8"/>
@@ -2741,7 +3548,7 @@
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>5</v>
@@ -2776,7 +3583,7 @@
       <c r="O23" s="8">
         <v>3</v>
       </c>
-      <c r="P23" s="36">
+      <c r="P23" s="35">
         <v>10</v>
       </c>
       <c r="Q23" s="8"/>
@@ -2786,7 +3593,7 @@
       <c r="S23" s="8">
         <v>0</v>
       </c>
-      <c r="T23" s="36">
+      <c r="T23" s="35">
         <v>2</v>
       </c>
       <c r="U23" s="8"/>
@@ -2808,7 +3615,7 @@
       <c r="AB23" s="9"/>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A24" s="25"/>
+      <c r="A24" s="24"/>
       <c r="B24" s="4" t="s">
         <v>6</v>
       </c>
@@ -2842,7 +3649,7 @@
       <c r="O24" s="8">
         <v>2</v>
       </c>
-      <c r="P24" s="36">
+      <c r="P24" s="35">
         <v>10</v>
       </c>
       <c r="Q24" s="8"/>
@@ -2852,7 +3659,7 @@
       <c r="S24" s="8">
         <v>0</v>
       </c>
-      <c r="T24" s="36">
+      <c r="T24" s="35">
         <v>3</v>
       </c>
       <c r="U24" s="8"/>
@@ -2908,7 +3715,7 @@
       <c r="O25" s="8">
         <v>6</v>
       </c>
-      <c r="P25" s="36">
+      <c r="P25" s="35">
         <v>20</v>
       </c>
       <c r="Q25" s="8"/>
@@ -2918,7 +3725,7 @@
       <c r="S25" s="8">
         <v>0</v>
       </c>
-      <c r="T25" s="36">
+      <c r="T25" s="35">
         <v>5</v>
       </c>
       <c r="U25" s="8"/>
@@ -2954,7 +3761,7 @@
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>5</v>
@@ -3144,7 +3951,7 @@
       </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A31" s="14"/>
+      <c r="A31" s="38"/>
     </row>
     <row r="32" spans="1:28" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G32" s="1"/>
@@ -3158,141 +3965,141 @@
       <c r="A33" s="6"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="37"/>
+      <c r="A34" s="36"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="38"/>
-      <c r="G35" s="26"/>
+      <c r="A35" s="37"/>
+      <c r="G35" s="25"/>
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="19"/>
-      <c r="K35" s="26"/>
+      <c r="K35" s="25"/>
       <c r="L35" s="19"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="38"/>
-      <c r="G36" s="27"/>
+      <c r="A36" s="37"/>
+      <c r="G36" s="26"/>
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="13"/>
-      <c r="K36" s="27"/>
+      <c r="K36" s="26"/>
       <c r="L36" s="13"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="38"/>
-      <c r="G37" s="26"/>
+      <c r="A37" s="37"/>
+      <c r="G37" s="25"/>
       <c r="H37" s="19"/>
       <c r="I37" s="19"/>
       <c r="J37" s="19"/>
-      <c r="K37" s="26"/>
+      <c r="K37" s="25"/>
       <c r="L37" s="19"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="38"/>
-      <c r="G38" s="27"/>
+      <c r="A38" s="37"/>
+      <c r="G38" s="26"/>
       <c r="H38" s="19"/>
       <c r="I38" s="19"/>
       <c r="J38" s="13"/>
-      <c r="K38" s="27"/>
+      <c r="K38" s="26"/>
       <c r="L38" s="13"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" s="37"/>
-      <c r="G39" s="27"/>
+      <c r="A39" s="36"/>
+      <c r="G39" s="26"/>
       <c r="H39" s="20"/>
       <c r="I39" s="20"/>
       <c r="J39" s="18"/>
-      <c r="K39" s="27"/>
+      <c r="K39" s="26"/>
       <c r="L39" s="18"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40" s="38"/>
-      <c r="G40" s="26"/>
+      <c r="A40" s="37"/>
+      <c r="G40" s="25"/>
       <c r="H40" s="19"/>
       <c r="I40" s="19"/>
       <c r="J40" s="19"/>
-      <c r="K40" s="26"/>
+      <c r="K40" s="25"/>
       <c r="L40" s="19"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41" s="38"/>
-      <c r="G41" s="27"/>
+      <c r="A41" s="37"/>
+      <c r="G41" s="26"/>
       <c r="H41" s="19"/>
       <c r="I41" s="19"/>
       <c r="J41" s="13"/>
-      <c r="K41" s="27"/>
+      <c r="K41" s="26"/>
       <c r="L41" s="13"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="38"/>
-      <c r="G42" s="27"/>
+      <c r="A42" s="37"/>
+      <c r="G42" s="26"/>
       <c r="H42" s="19"/>
       <c r="I42" s="19"/>
       <c r="J42" s="13"/>
-      <c r="K42" s="27"/>
+      <c r="K42" s="26"/>
       <c r="L42" s="13"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="6"/>
-      <c r="G43" s="27"/>
+      <c r="G43" s="26"/>
       <c r="H43" s="18"/>
       <c r="I43" s="18"/>
       <c r="J43" s="18"/>
-      <c r="K43" s="27"/>
+      <c r="K43" s="26"/>
       <c r="L43" s="18"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A44" s="38"/>
-      <c r="G44" s="27"/>
+      <c r="A44" s="37"/>
+      <c r="G44" s="26"/>
       <c r="H44" s="13"/>
       <c r="I44" s="13"/>
       <c r="J44" s="13"/>
-      <c r="K44" s="27"/>
+      <c r="K44" s="26"/>
       <c r="L44" s="13"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A45" s="38"/>
-      <c r="G45" s="27"/>
+      <c r="A45" s="37"/>
+      <c r="G45" s="26"/>
       <c r="H45" s="13"/>
       <c r="I45" s="13"/>
       <c r="J45" s="13"/>
-      <c r="K45" s="27"/>
+      <c r="K45" s="26"/>
       <c r="L45" s="13"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="6"/>
-      <c r="G46" s="27"/>
+      <c r="G46" s="26"/>
       <c r="H46" s="18"/>
       <c r="I46" s="18"/>
       <c r="J46" s="18"/>
-      <c r="K46" s="27"/>
+      <c r="K46" s="26"/>
       <c r="L46" s="18"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A47" s="38"/>
-      <c r="G47" s="27"/>
+      <c r="A47" s="37"/>
+      <c r="G47" s="26"/>
       <c r="H47" s="13"/>
       <c r="I47" s="13"/>
       <c r="J47" s="13"/>
-      <c r="K47" s="27"/>
+      <c r="K47" s="26"/>
       <c r="L47" s="13"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A48" s="38"/>
-      <c r="G48" s="27"/>
+      <c r="A48" s="37"/>
+      <c r="G48" s="26"/>
       <c r="H48" s="13"/>
       <c r="I48" s="13"/>
       <c r="J48" s="13"/>
-      <c r="K48" s="27"/>
+      <c r="K48" s="26"/>
       <c r="L48" s="13"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A49" s="38"/>
-      <c r="G49" s="27"/>
+      <c r="A49" s="37"/>
+      <c r="G49" s="26"/>
       <c r="H49" s="13"/>
       <c r="I49" s="13"/>
       <c r="J49" s="13"/>
-      <c r="K49" s="27"/>
+      <c r="K49" s="26"/>
       <c r="L49" s="13"/>
     </row>
     <row r="50" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
finished refactoring simulate.py (hopefully)
</commit_message>
<xml_diff>
--- a/doc/excel-skabalon.xlsx
+++ b/doc/excel-skabalon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonasson/voting/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01CCF48C-F532-CB49-81DB-632F0BC461D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB61DDE7-1E6A-1446-B2C4-B87B892C823E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4960" yWindow="-20940" windowWidth="38420" windowHeight="20900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4660" yWindow="-20940" windowWidth="38400" windowHeight="20900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Common settings" sheetId="2" r:id="rId1"/>
@@ -1587,13 +1587,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748E841B-6C29-834D-9376-1530C4084D09}">
-  <dimension ref="A1:AB38"/>
+  <dimension ref="A1:AB39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="172" zoomScaleNormal="142" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomRight" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2167,8 +2167,9 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="27" t="s">
-        <v>56</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="B20" s="40"/>
       <c r="C20" s="48"/>
       <c r="D20" s="48"/>
       <c r="E20" s="48"/>
@@ -2182,194 +2183,158 @@
       <c r="O20" s="39"/>
       <c r="P20" s="39"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A21" s="53" t="s">
+    <row r="21" spans="1:21" s="22" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21" s="51">
-        <v>0.121</v>
-      </c>
-      <c r="E21" s="51">
-        <v>0.44606235918925974</v>
-      </c>
-      <c r="F21" s="51">
-        <v>3.6810559144514143E-2</v>
-      </c>
-      <c r="H21" s="50">
-        <v>0</v>
-      </c>
-      <c r="I21" s="50">
-        <v>0</v>
-      </c>
-      <c r="J21" s="50">
-        <v>0</v>
-      </c>
-      <c r="K21" s="50">
+      <c r="B21" s="45"/>
+      <c r="C21" s="44">
+        <v>7.3345721486019477E-2</v>
+      </c>
+      <c r="D21" s="44">
+        <v>0.37588227455947576</v>
+      </c>
+      <c r="E21" s="44">
+        <v>0.37588227455947576</v>
+      </c>
+      <c r="F21" s="44">
+        <v>5.0892136616471073E-2</v>
+      </c>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43">
+        <v>0</v>
+      </c>
+      <c r="I21" s="43">
         <v>1</v>
       </c>
-      <c r="L21" s="50"/>
-      <c r="M21" s="50">
-        <v>0</v>
-      </c>
-      <c r="N21" s="50">
+      <c r="J21" s="43">
+        <v>0</v>
+      </c>
+      <c r="K21" s="43">
+        <v>0</v>
+      </c>
+      <c r="L21" s="42"/>
+      <c r="M21" s="43">
+        <v>2</v>
+      </c>
+      <c r="N21" s="43">
+        <v>1</v>
+      </c>
+      <c r="O21" s="43">
         <v>3</v>
       </c>
-      <c r="O21" s="50">
-        <v>2</v>
-      </c>
-      <c r="P21" s="50">
+      <c r="P21" s="43">
+        <v>3</v>
+      </c>
+      <c r="Q21" s="42"/>
+    </row>
+    <row r="22" spans="1:21" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="45"/>
+      <c r="C22" s="44">
+        <v>0.83021769396323619</v>
+      </c>
+      <c r="D22" s="44">
+        <v>0.90006631200155518</v>
+      </c>
+      <c r="E22" s="44">
+        <v>0.90006631200155518</v>
+      </c>
+      <c r="F22" s="44">
+        <v>0.5962960523233668</v>
+      </c>
+      <c r="G22" s="42"/>
+      <c r="H22" s="43">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B22" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="48">
-        <v>0.121</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22" s="48" t="s">
-        <v>55</v>
-      </c>
-      <c r="F22">
-        <v>0.89300000000000002</v>
-      </c>
-      <c r="H22" s="39">
-        <v>0</v>
-      </c>
-      <c r="I22" s="39">
-        <v>0</v>
-      </c>
-      <c r="J22" s="39">
-        <v>0</v>
-      </c>
-      <c r="K22" s="39">
+      <c r="I22" s="43">
+        <v>0</v>
+      </c>
+      <c r="J22" s="43">
         <v>1</v>
       </c>
-      <c r="M22" s="39">
+      <c r="K22" s="43">
+        <v>1</v>
+      </c>
+      <c r="L22" s="42"/>
+      <c r="M22" s="43">
+        <v>1</v>
+      </c>
+      <c r="N22" s="43">
+        <v>2</v>
+      </c>
+      <c r="O22" s="43">
         <v>3</v>
       </c>
-      <c r="N22" s="39">
-        <v>0</v>
-      </c>
-      <c r="O22" s="39">
+      <c r="P22" s="43">
         <v>3</v>
       </c>
-      <c r="P22" s="39">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B23" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" s="48">
-        <v>3.6810559144514143E-2</v>
-      </c>
-      <c r="D23" s="48">
-        <v>0.8932948068518588</v>
-      </c>
-      <c r="E23">
-        <v>0.21299999999999999</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-      <c r="I23">
-        <v>1</v>
-      </c>
-      <c r="J23">
-        <v>1</v>
-      </c>
-      <c r="K23" s="39">
-        <v>0</v>
-      </c>
-      <c r="M23">
-        <v>1</v>
-      </c>
-      <c r="N23">
-        <v>2</v>
-      </c>
-      <c r="O23">
-        <v>3</v>
-      </c>
-      <c r="P23" s="39">
-        <v>0</v>
-      </c>
+      <c r="Q22" s="42"/>
+      <c r="R22" s="41"/>
+      <c r="S22" s="41"/>
+      <c r="T22" s="41"/>
+      <c r="U22" s="41"/>
+    </row>
+    <row r="23" spans="1:21" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="46"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43"/>
+      <c r="K23" s="43"/>
+      <c r="L23" s="42"/>
+      <c r="M23" s="43"/>
+      <c r="N23" s="43"/>
+      <c r="O23" s="43"/>
+      <c r="P23" s="43"/>
+      <c r="Q23" s="42"/>
+      <c r="R23" s="41"/>
+      <c r="S23" s="41"/>
+      <c r="T23" s="41"/>
+      <c r="U23" s="41"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B24" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="48" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24" s="48" t="s">
-        <v>53</v>
-      </c>
-      <c r="E24" s="48" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="48" t="s">
-        <v>53</v>
-      </c>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="I24" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="J24" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="K24" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="L24" s="39"/>
-      <c r="M24" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="N24" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="O24" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="P24" s="39" t="s">
-        <v>53</v>
-      </c>
+      <c r="A24" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="48"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="39"/>
+      <c r="M24" s="39"/>
+      <c r="N24" s="39"/>
+      <c r="O24" s="39"/>
+      <c r="P24" s="39"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A25" s="52" t="s">
-        <v>48</v>
+      <c r="A25" s="53" t="s">
+        <v>44</v>
       </c>
       <c r="B25" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="49">
+      <c r="C25">
         <v>0</v>
       </c>
       <c r="D25" s="51">
-        <v>0.34612668354933307</v>
+        <v>0.121</v>
       </c>
       <c r="E25" s="51">
-        <v>0.23100000000000001</v>
+        <v>0.44606235918925974</v>
       </c>
       <c r="F25" s="51">
-        <v>0.49345681797586316</v>
+        <v>3.6810559144514143E-2</v>
       </c>
       <c r="H25" s="50">
         <v>0</v>
@@ -2378,23 +2343,23 @@
         <v>0</v>
       </c>
       <c r="J25" s="50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K25" s="50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L25" s="50"/>
       <c r="M25" s="50">
         <v>0</v>
       </c>
       <c r="N25" s="50">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O25" s="50">
         <v>2</v>
       </c>
       <c r="P25" s="50">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.2">
@@ -2402,41 +2367,40 @@
         <v>51</v>
       </c>
       <c r="C26" s="48">
-        <v>0.34612668354933307</v>
-      </c>
-      <c r="D26" s="49">
-        <v>0</v>
-      </c>
-      <c r="E26" s="48">
-        <v>2.4569999999999999</v>
-      </c>
-      <c r="F26" s="48">
-        <v>0.84699999999999998</v>
-      </c>
-      <c r="H26" s="49">
-        <v>0</v>
-      </c>
-      <c r="I26" s="49">
-        <v>0</v>
-      </c>
-      <c r="J26" s="49">
-        <v>2</v>
-      </c>
-      <c r="K26" s="49">
+        <v>0.121</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="F26">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="H26" s="39">
+        <v>0</v>
+      </c>
+      <c r="I26" s="39">
+        <v>0</v>
+      </c>
+      <c r="J26" s="39">
+        <v>0</v>
+      </c>
+      <c r="K26" s="39">
         <v>1</v>
       </c>
-      <c r="L26" s="50"/>
-      <c r="M26" s="49">
-        <v>2</v>
-      </c>
-      <c r="N26" s="49">
-        <v>0</v>
-      </c>
-      <c r="O26" s="49">
-        <v>2</v>
-      </c>
-      <c r="P26" s="49">
+      <c r="M26" s="39">
         <v>3</v>
+      </c>
+      <c r="N26" s="39">
+        <v>0</v>
+      </c>
+      <c r="O26" s="39">
+        <v>3</v>
+      </c>
+      <c r="P26" s="39">
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.2">
@@ -2444,209 +2408,268 @@
         <v>50</v>
       </c>
       <c r="C27" s="48">
+        <v>3.6810559144514143E-2</v>
+      </c>
+      <c r="D27" s="48">
+        <v>0.8932948068518588</v>
+      </c>
+      <c r="E27">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27" s="39">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <v>2</v>
+      </c>
+      <c r="O27">
+        <v>3</v>
+      </c>
+      <c r="P27" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B28" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="I28" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="J28" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="K28" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="L28" s="39"/>
+      <c r="M28" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="N28" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="O28" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="P28" s="39" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A29" s="52" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="49">
+        <v>0</v>
+      </c>
+      <c r="D29" s="51">
+        <v>0.34612668354933307</v>
+      </c>
+      <c r="E29" s="51">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="F29" s="51">
         <v>0.49345681797586316</v>
       </c>
-      <c r="D27" s="48">
+      <c r="H29" s="50">
+        <v>0</v>
+      </c>
+      <c r="I29" s="50">
+        <v>0</v>
+      </c>
+      <c r="J29" s="50">
+        <v>2</v>
+      </c>
+      <c r="K29" s="50">
+        <v>0</v>
+      </c>
+      <c r="L29" s="50"/>
+      <c r="M29" s="50">
+        <v>0</v>
+      </c>
+      <c r="N29" s="50">
+        <v>2</v>
+      </c>
+      <c r="O29" s="50">
+        <v>2</v>
+      </c>
+      <c r="P29" s="50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B30" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="48">
+        <v>0.34612668354933307</v>
+      </c>
+      <c r="D30" s="49">
+        <v>0</v>
+      </c>
+      <c r="E30" s="48">
+        <v>2.4569999999999999</v>
+      </c>
+      <c r="F30" s="48">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="H30" s="49">
+        <v>0</v>
+      </c>
+      <c r="I30" s="49">
+        <v>0</v>
+      </c>
+      <c r="J30" s="49">
+        <v>2</v>
+      </c>
+      <c r="K30" s="49">
+        <v>1</v>
+      </c>
+      <c r="L30" s="50"/>
+      <c r="M30" s="49">
+        <v>2</v>
+      </c>
+      <c r="N30" s="49">
+        <v>0</v>
+      </c>
+      <c r="O30" s="49">
+        <v>2</v>
+      </c>
+      <c r="P30" s="49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B31" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="48">
+        <v>0.49345681797586316</v>
+      </c>
+      <c r="D31" s="48">
         <v>0.84746134572101128</v>
       </c>
-      <c r="E27" s="48">
+      <c r="E31" s="48">
         <v>2.4565424329266676</v>
       </c>
-      <c r="F27" s="49">
-        <v>0</v>
-      </c>
-      <c r="H27" s="49">
-        <v>0</v>
-      </c>
-      <c r="I27" s="49">
+      <c r="F31" s="49">
+        <v>0</v>
+      </c>
+      <c r="H31" s="49">
+        <v>0</v>
+      </c>
+      <c r="I31" s="49">
         <v>1</v>
       </c>
-      <c r="J27" s="49">
-        <v>0</v>
-      </c>
-      <c r="K27" s="49">
-        <v>0</v>
-      </c>
-      <c r="L27" s="50"/>
-      <c r="M27" s="49">
+      <c r="J31" s="49">
+        <v>0</v>
+      </c>
+      <c r="K31" s="49">
+        <v>0</v>
+      </c>
+      <c r="L31" s="50"/>
+      <c r="M31" s="49">
         <v>3</v>
       </c>
-      <c r="N27" s="49">
+      <c r="N31" s="49">
         <v>3</v>
       </c>
-      <c r="O27" s="49">
+      <c r="O31" s="49">
         <v>4</v>
       </c>
-      <c r="P27" s="49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B28" s="14"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="39"/>
-      <c r="K28" s="39"/>
-      <c r="M28" s="39"/>
-      <c r="N28" s="39"/>
-      <c r="O28" s="39"/>
-      <c r="P28" s="39"/>
-      <c r="R28" s="39"/>
-      <c r="S28" s="39"/>
-      <c r="T28" s="39"/>
-      <c r="U28" s="39"/>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A29" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="48"/>
-      <c r="D29" s="48"/>
-      <c r="E29" s="48"/>
-      <c r="F29" s="48"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="M29" s="39"/>
-      <c r="N29" s="39"/>
-      <c r="O29" s="39"/>
-      <c r="P29" s="39"/>
-    </row>
-    <row r="30" spans="1:21" s="22" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="44">
-        <v>7.3345721486019477E-2</v>
-      </c>
-      <c r="D30" s="44">
-        <v>0.37588227455947576</v>
-      </c>
-      <c r="E30" s="44">
-        <v>0.37588227455947576</v>
-      </c>
-      <c r="F30" s="44">
-        <v>5.0892136616471073E-2</v>
-      </c>
-      <c r="G30" s="43"/>
-      <c r="H30" s="43">
-        <v>0</v>
-      </c>
-      <c r="I30" s="43">
-        <v>1</v>
-      </c>
-      <c r="J30" s="43">
-        <v>0</v>
-      </c>
-      <c r="K30" s="43">
-        <v>0</v>
-      </c>
-      <c r="L30" s="42"/>
-      <c r="M30" s="43">
-        <v>2</v>
-      </c>
-      <c r="N30" s="43">
-        <v>1</v>
-      </c>
-      <c r="O30" s="43">
-        <v>3</v>
-      </c>
-      <c r="P30" s="43">
-        <v>3</v>
-      </c>
-      <c r="Q30" s="42"/>
-    </row>
-    <row r="31" spans="1:21" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="46" t="s">
-        <v>48</v>
-      </c>
-      <c r="B31" s="45"/>
-      <c r="C31" s="44">
-        <v>0.83021769396323619</v>
-      </c>
-      <c r="D31" s="44">
-        <v>0.90006631200155518</v>
-      </c>
-      <c r="E31" s="44">
-        <v>0.90006631200155518</v>
-      </c>
-      <c r="F31" s="44">
-        <v>0.5962960523233668</v>
-      </c>
-      <c r="G31" s="42"/>
-      <c r="H31" s="43">
-        <v>1</v>
-      </c>
-      <c r="I31" s="43">
-        <v>0</v>
-      </c>
-      <c r="J31" s="43">
-        <v>1</v>
-      </c>
-      <c r="K31" s="43">
-        <v>1</v>
-      </c>
-      <c r="L31" s="42"/>
-      <c r="M31" s="43">
-        <v>1</v>
-      </c>
-      <c r="N31" s="43">
-        <v>2</v>
-      </c>
-      <c r="O31" s="43">
-        <v>3</v>
-      </c>
-      <c r="P31" s="43">
-        <v>3</v>
-      </c>
-      <c r="Q31" s="42"/>
-      <c r="R31" s="41"/>
-      <c r="S31" s="41"/>
-      <c r="T31" s="41"/>
-      <c r="U31" s="41"/>
-    </row>
-    <row r="32" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P31" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B32" s="14"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="39"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="39"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="39"/>
+      <c r="M32" s="39"/>
+      <c r="N32" s="39"/>
+      <c r="O32" s="39"/>
+      <c r="P32" s="39"/>
       <c r="R32" s="39"/>
       <c r="S32" s="39"/>
       <c r="T32" s="39"/>
       <c r="U32" s="39"/>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R33" s="39"/>
       <c r="S33" s="39"/>
       <c r="T33" s="39"/>
       <c r="U33" s="39"/>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A35" s="40" t="s">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="R34" s="39"/>
+      <c r="S34" s="39"/>
+      <c r="T34" s="39"/>
+      <c r="U34" s="39"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A36" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C35" s="39">
-        <v>0</v>
-      </c>
-      <c r="D35" s="39">
-        <v>0</v>
-      </c>
-      <c r="E35" s="39">
-        <v>0</v>
-      </c>
-      <c r="F35" s="39">
-        <v>0</v>
-      </c>
-      <c r="R35" s="39"/>
-      <c r="S35" s="39"/>
-      <c r="T35" s="39"/>
-      <c r="U35" s="39"/>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A38" s="27"/>
+      <c r="C36" s="39">
+        <v>0</v>
+      </c>
+      <c r="D36" s="39">
+        <v>0</v>
+      </c>
+      <c r="E36" s="39">
+        <v>0</v>
+      </c>
+      <c r="F36" s="39">
+        <v>0</v>
+      </c>
+      <c r="R36" s="39"/>
+      <c r="S36" s="39"/>
+      <c r="T36" s="39"/>
+      <c r="U36" s="39"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A39" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>